<commit_message>
updates to program and specs Feb 22 2023
</commit_message>
<xml_diff>
--- a/metadata/specs.xlsx
+++ b/metadata/specs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neitmant/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brolleyb\Documents\Admiral_Hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACC596A-F463-E147-829A-71860B7FE1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3F14066-47DF-44C6-AAF6-CE9F8D374460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define" sheetId="1" r:id="rId1"/>
@@ -44,8 +44,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -5431,11 +5435,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5523,7 +5534,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5560,6 +5571,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -5580,41 +5597,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5837,11 +5856,11 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="74.33203125" customWidth="1"/>
-    <col min="3" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="3" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6891,12 +6910,12 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="62.5" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -7920,10 +7939,10 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -8939,19 +8958,19 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="46.83203125" customWidth="1"/>
-    <col min="5" max="6" width="19.5" customWidth="1"/>
+    <col min="1" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1"/>
+    <col min="5" max="6" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="82" customWidth="1"/>
-    <col min="8" max="9" width="19.5" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" customWidth="1"/>
-    <col min="11" max="12" width="19.5" customWidth="1"/>
-    <col min="13" max="13" width="27.33203125" customWidth="1"/>
-    <col min="14" max="14" width="19.5" customWidth="1"/>
-    <col min="15" max="26" width="8.6640625" customWidth="1"/>
+    <col min="8" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+    <col min="11" max="12" width="19.42578125" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" customWidth="1"/>
+    <col min="15" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -9997,18 +10016,18 @@
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" customWidth="1"/>
-    <col min="4" max="4" width="66.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.5" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
-    <col min="10" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -11224,25 +11243,25 @@
       <selection pane="bottomLeft" activeCell="A272" sqref="A272:XFD272"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="3" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.33203125" customWidth="1"/>
-    <col min="17" max="19" width="15.5" customWidth="1"/>
-    <col min="20" max="26" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="17" max="19" width="15.42578125" customWidth="1"/>
+    <col min="20" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -22878,24 +22897,24 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="13" width="12.83203125" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.33203125" customWidth="1"/>
-    <col min="17" max="18" width="15.5" customWidth="1"/>
-    <col min="19" max="26" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="17" max="18" width="15.42578125" customWidth="1"/>
+    <col min="19" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -23955,17 +23974,17 @@
       <selection pane="bottomRight" activeCell="B383" sqref="B383"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -34245,12 +34264,12 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -35300,20 +35319,20 @@
   <dimension ref="A1:H790"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
+      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D213" sqref="D213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
-    <col min="4" max="4" width="46.83203125" customWidth="1"/>
-    <col min="5" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -35342,7 +35361,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16" hidden="1">
+    <row r="2" spans="1:8" hidden="1">
       <c r="A2" s="2" t="s">
         <v>236</v>
       </c>
@@ -35356,7 +35375,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" hidden="1">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="2" t="s">
         <v>239</v>
       </c>
@@ -35370,7 +35389,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" hidden="1">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="2" t="s">
         <v>316</v>
       </c>
@@ -35384,7 +35403,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" hidden="1">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" s="2" t="s">
         <v>272</v>
       </c>
@@ -35398,7 +35417,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16" hidden="1">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="2" t="s">
         <v>253</v>
       </c>
@@ -35412,7 +35431,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" hidden="1">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" s="2" t="s">
         <v>265</v>
       </c>
@@ -35426,7 +35445,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16" hidden="1">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="2" t="s">
         <v>268</v>
       </c>
@@ -35440,7 +35459,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" hidden="1">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="2" t="s">
         <v>259</v>
       </c>
@@ -35454,7 +35473,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16" hidden="1">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="2" t="s">
         <v>262</v>
       </c>
@@ -35468,7 +35487,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16" hidden="1">
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" s="2" t="s">
         <v>247</v>
       </c>
@@ -35482,7 +35501,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16" hidden="1">
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" s="2" t="s">
         <v>250</v>
       </c>
@@ -35496,7 +35515,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16" hidden="1">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="2" t="s">
         <v>230</v>
       </c>
@@ -35510,7 +35529,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="32" hidden="1">
+    <row r="14" spans="1:8" ht="45" hidden="1">
       <c r="A14" s="2" t="s">
         <v>233</v>
       </c>
@@ -35524,7 +35543,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16" hidden="1">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="2" t="s">
         <v>321</v>
       </c>
@@ -35930,7 +35949,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="96" hidden="1">
+    <row r="44" spans="1:4" ht="105" hidden="1">
       <c r="A44" s="2" t="s">
         <v>355</v>
       </c>
@@ -36112,7 +36131,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1">
+    <row r="57" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>407</v>
       </c>
@@ -36126,7 +36145,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1">
+    <row r="58" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>404</v>
       </c>
@@ -36140,7 +36159,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1">
+    <row r="59" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>431</v>
       </c>
@@ -36154,7 +36173,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1">
+    <row r="60" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>386</v>
       </c>
@@ -36168,7 +36187,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1">
+    <row r="61" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>385</v>
       </c>
@@ -36182,7 +36201,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1">
+    <row r="62" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>434</v>
       </c>
@@ -36196,7 +36215,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1">
+    <row r="63" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>372</v>
       </c>
@@ -36210,7 +36229,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1">
+    <row r="64" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A64" s="2" t="s">
         <v>373</v>
       </c>
@@ -36224,7 +36243,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1">
+    <row r="65" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>374</v>
       </c>
@@ -36238,7 +36257,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1">
+    <row r="66" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>423</v>
       </c>
@@ -36252,7 +36271,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1">
+    <row r="67" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>420</v>
       </c>
@@ -36266,7 +36285,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="224">
+    <row r="68" spans="1:4" ht="255" hidden="1">
       <c r="A68" s="2" t="s">
         <v>427</v>
       </c>
@@ -36280,7 +36299,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1">
+    <row r="69" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A69" s="2" t="s">
         <v>399</v>
       </c>
@@ -36294,7 +36313,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1">
+    <row r="70" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A70" s="2" t="s">
         <v>383</v>
       </c>
@@ -36308,7 +36327,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1">
+    <row r="71" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>384</v>
       </c>
@@ -36322,7 +36341,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1">
+    <row r="72" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>400</v>
       </c>
@@ -36336,7 +36355,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1">
+    <row r="73" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>430</v>
       </c>
@@ -36350,7 +36369,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1">
+    <row r="74" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>419</v>
       </c>
@@ -36364,7 +36383,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1">
+    <row r="75" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>416</v>
       </c>
@@ -36378,7 +36397,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1">
+    <row r="76" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>401</v>
       </c>
@@ -36392,7 +36411,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1">
+    <row r="77" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>378</v>
       </c>
@@ -36406,7 +36425,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1">
+    <row r="78" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A78" s="2" t="s">
         <v>381</v>
       </c>
@@ -36420,7 +36439,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1">
+    <row r="79" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>439</v>
       </c>
@@ -36434,7 +36453,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1">
+    <row r="80" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A80" s="2" t="s">
         <v>436</v>
       </c>
@@ -36448,7 +36467,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1">
+    <row r="81" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>442</v>
       </c>
@@ -36462,7 +36481,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1">
+    <row r="82" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A82" s="2" t="s">
         <v>390</v>
       </c>
@@ -36476,7 +36495,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1">
+    <row r="83" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>392</v>
       </c>
@@ -36490,7 +36509,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1">
+    <row r="84" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A84" s="2" t="s">
         <v>394</v>
       </c>
@@ -36504,7 +36523,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1">
+    <row r="85" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>398</v>
       </c>
@@ -36518,7 +36537,7 @@
         <v>1698</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1">
+    <row r="86" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A86" s="2" t="s">
         <v>413</v>
       </c>
@@ -36532,7 +36551,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1">
+    <row r="87" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A87" s="2" t="s">
         <v>410</v>
       </c>
@@ -36546,7 +36565,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1">
+    <row r="88" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A88" s="2" t="s">
         <v>375</v>
       </c>
@@ -36560,7 +36579,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1">
+    <row r="89" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A89" s="2" t="s">
         <v>376</v>
       </c>
@@ -36574,7 +36593,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1">
+    <row r="90" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A90" s="2" t="s">
         <v>382</v>
       </c>
@@ -36588,7 +36607,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1">
+    <row r="91" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A91" s="2" t="s">
         <v>377</v>
       </c>
@@ -36602,7 +36621,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1">
+    <row r="92" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A92" s="2" t="s">
         <v>361</v>
       </c>
@@ -36616,7 +36635,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1">
+    <row r="93" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A93" s="2" t="s">
         <v>364</v>
       </c>
@@ -36630,7 +36649,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1">
+    <row r="94" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A94" s="2" t="s">
         <v>368</v>
       </c>
@@ -36644,7 +36663,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1">
+    <row r="95" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A95" s="2" t="s">
         <v>369</v>
       </c>
@@ -36658,7 +36677,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1">
+    <row r="96" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A96" s="2" t="s">
         <v>371</v>
       </c>
@@ -36672,7 +36691,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1">
+    <row r="97" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A97" s="2" t="s">
         <v>366</v>
       </c>
@@ -36686,7 +36705,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1">
+    <row r="98" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A98" s="2" t="s">
         <v>367</v>
       </c>
@@ -36700,7 +36719,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1">
+    <row r="99" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A99" s="2" t="s">
         <v>370</v>
       </c>
@@ -36714,7 +36733,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1">
+    <row r="100" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A100" s="2" t="s">
         <v>365</v>
       </c>
@@ -36728,7 +36747,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1">
+    <row r="101" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A101" s="2" t="s">
         <v>387</v>
       </c>
@@ -36742,7 +36761,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1">
+    <row r="102" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A102" s="2" t="s">
         <v>388</v>
       </c>
@@ -38002,8 +38021,8 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A192" s="2" t="s">
+    <row r="192" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A192" s="20" t="s">
         <v>583</v>
       </c>
       <c r="B192" s="2" t="s">
@@ -38016,8 +38035,8 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A193" s="2" t="s">
+    <row r="193" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A193" s="20" t="s">
         <v>584</v>
       </c>
       <c r="B193" s="2" t="s">
@@ -38030,8 +38049,8 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A194" s="2" t="s">
+    <row r="194" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A194" s="20" t="s">
         <v>585</v>
       </c>
       <c r="B194" s="2" t="s">
@@ -38044,8 +38063,8 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A195" s="2" t="s">
+    <row r="195" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A195" s="20" t="s">
         <v>588</v>
       </c>
       <c r="B195" s="2" t="s">
@@ -38058,8 +38077,8 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A196" s="2" t="s">
+    <row r="196" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A196" s="20" t="s">
         <v>559</v>
       </c>
       <c r="B196" s="2" t="s">
@@ -38072,7 +38091,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="197" spans="1:4" ht="15.75" customHeight="1">
       <c r="A197" s="2" t="s">
         <v>579</v>
       </c>
@@ -38086,8 +38105,8 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A198" s="2" t="s">
+    <row r="198" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A198" s="20" t="s">
         <v>615</v>
       </c>
       <c r="B198" s="2" t="s">
@@ -38100,8 +38119,8 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A199" s="2" t="s">
+    <row r="199" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A199" s="20" t="s">
         <v>619</v>
       </c>
       <c r="B199" s="2" t="s">
@@ -38114,7 +38133,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="200" spans="1:4" ht="15.75" customHeight="1">
       <c r="A200" s="2" t="s">
         <v>604</v>
       </c>
@@ -38128,7 +38147,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="201" spans="1:4" ht="15.75" customHeight="1">
       <c r="A201" s="2" t="s">
         <v>605</v>
       </c>
@@ -38142,7 +38161,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="32" hidden="1">
+    <row r="202" spans="1:4" ht="30">
       <c r="A202" s="2" t="s">
         <v>601</v>
       </c>
@@ -38156,7 +38175,7 @@
         <v>1693</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="176" hidden="1">
+    <row r="203" spans="1:4" ht="180">
       <c r="A203" s="2" t="s">
         <v>582</v>
       </c>
@@ -38170,8 +38189,8 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A204" s="2" t="s">
+    <row r="204" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A204" s="20" t="s">
         <v>657</v>
       </c>
       <c r="B204" s="2" t="s">
@@ -38184,8 +38203,8 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A205" s="2" t="s">
+    <row r="205" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A205" s="20" t="s">
         <v>664</v>
       </c>
       <c r="B205" s="2" t="s">
@@ -38198,8 +38217,8 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A206" s="2" t="s">
+    <row r="206" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A206" s="20" t="s">
         <v>608</v>
       </c>
       <c r="B206" s="2" t="s">
@@ -38212,8 +38231,8 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A207" s="2" t="s">
+    <row r="207" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A207" s="20" t="s">
         <v>631</v>
       </c>
       <c r="B207" s="2" t="s">
@@ -38226,8 +38245,8 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A208" s="2" t="s">
+    <row r="208" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A208" s="20" t="s">
         <v>609</v>
       </c>
       <c r="B208" s="2" t="s">
@@ -38240,8 +38259,8 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A209" s="2" t="s">
+    <row r="209" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A209" s="20" t="s">
         <v>612</v>
       </c>
       <c r="B209" s="2" t="s">
@@ -38254,8 +38273,8 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A210" s="2" t="s">
+    <row r="210" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A210" s="20" t="s">
         <v>634</v>
       </c>
       <c r="B210" s="2" t="s">
@@ -38268,8 +38287,8 @@
         <v>1689</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A211" s="2" t="s">
+    <row r="211" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A211" s="20" t="s">
         <v>638</v>
       </c>
       <c r="B211" s="2" t="s">
@@ -38282,8 +38301,8 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A212" s="2" t="s">
+    <row r="212" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A212" s="20" t="s">
         <v>628</v>
       </c>
       <c r="B212" s="2" t="s">
@@ -38296,7 +38315,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="213" spans="1:4" ht="15.75" customHeight="1">
       <c r="A213" s="2" t="s">
         <v>598</v>
       </c>
@@ -38310,8 +38329,8 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A214" s="2" t="s">
+    <row r="214" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A214" s="20" t="s">
         <v>660</v>
       </c>
       <c r="B214" s="2" t="s">
@@ -38324,8 +38343,8 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A215" s="2" t="s">
+    <row r="215" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A215" s="20" t="s">
         <v>594</v>
       </c>
       <c r="B215" s="2" t="s">
@@ -38338,8 +38357,8 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A216" s="2" t="s">
+    <row r="216" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A216" s="20" t="s">
         <v>622</v>
       </c>
       <c r="B216" s="2" t="s">
@@ -38352,8 +38371,8 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A217" s="2" t="s">
+    <row r="217" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A217" s="20" t="s">
         <v>597</v>
       </c>
       <c r="B217" s="2" t="s">
@@ -38366,8 +38385,8 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A218" s="2" t="s">
+    <row r="218" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A218" s="20" t="s">
         <v>667</v>
       </c>
       <c r="B218" s="2" t="s">
@@ -38380,8 +38399,8 @@
         <v>1688</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A219" s="2" t="s">
+    <row r="219" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A219" s="20" t="s">
         <v>589</v>
       </c>
       <c r="B219" s="2" t="s">
@@ -38394,8 +38413,8 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A220" s="2" t="s">
+    <row r="220" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A220" s="20" t="s">
         <v>590</v>
       </c>
       <c r="B220" s="2" t="s">
@@ -38408,8 +38427,8 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A221" s="2" t="s">
+    <row r="221" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A221" s="20" t="s">
         <v>653</v>
       </c>
       <c r="B221" s="2" t="s">
@@ -38422,8 +38441,8 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A222" s="2" t="s">
+    <row r="222" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A222" s="20" t="s">
         <v>647</v>
       </c>
       <c r="B222" s="2" t="s">
@@ -38436,8 +38455,8 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A223" s="2" t="s">
+    <row r="223" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A223" s="20" t="s">
         <v>644</v>
       </c>
       <c r="B223" s="2" t="s">
@@ -38450,8 +38469,8 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A224" s="2" t="s">
+    <row r="224" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A224" s="20" t="s">
         <v>595</v>
       </c>
       <c r="B224" s="2" t="s">
@@ -38464,8 +38483,8 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A225" s="2" t="s">
+    <row r="225" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A225" s="20" t="s">
         <v>591</v>
       </c>
       <c r="B225" s="2" t="s">
@@ -38478,8 +38497,8 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A226" s="2" t="s">
+    <row r="226" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A226" s="20" t="s">
         <v>557</v>
       </c>
       <c r="B226" s="2" t="s">
@@ -38492,8 +38511,8 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A227" s="2" t="s">
+    <row r="227" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A227" s="20" t="s">
         <v>556</v>
       </c>
       <c r="B227" s="2" t="s">
@@ -38506,8 +38525,8 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A228" s="2" t="s">
+    <row r="228" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A228" s="20" t="s">
         <v>553</v>
       </c>
       <c r="B228" s="2" t="s">
@@ -38520,8 +38539,8 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A229" s="2" t="s">
+    <row r="229" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A229" s="20" t="s">
         <v>555</v>
       </c>
       <c r="B229" s="2" t="s">
@@ -38534,8 +38553,8 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A230" s="2" t="s">
+    <row r="230" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A230" s="20" t="s">
         <v>568</v>
       </c>
       <c r="B230" s="2" t="s">
@@ -38548,8 +38567,8 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A231" s="2" t="s">
+    <row r="231" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A231" s="20" t="s">
         <v>571</v>
       </c>
       <c r="B231" s="2" t="s">
@@ -38562,8 +38581,8 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A232" s="2" t="s">
+    <row r="232" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A232" s="20" t="s">
         <v>562</v>
       </c>
       <c r="B232" s="2" t="s">
@@ -38576,8 +38595,8 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A233" s="2" t="s">
+    <row r="233" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A233" s="20" t="s">
         <v>565</v>
       </c>
       <c r="B233" s="2" t="s">
@@ -38590,8 +38609,8 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A234" s="2" t="s">
+    <row r="234" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A234" s="20" t="s">
         <v>576</v>
       </c>
       <c r="B234" s="2" t="s">
@@ -38604,8 +38623,8 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A235" s="2" t="s">
+    <row r="235" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A235" s="20" t="s">
         <v>573</v>
       </c>
       <c r="B235" s="2" t="s">
@@ -38618,8 +38637,8 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A236" s="2" t="s">
+    <row r="236" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A236" s="20" t="s">
         <v>572</v>
       </c>
       <c r="B236" s="2" t="s">
@@ -38632,8 +38651,8 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A237" s="2" t="s">
+    <row r="237" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A237" s="21" t="s">
         <v>554</v>
       </c>
       <c r="B237" s="2" t="s">
@@ -38646,8 +38665,8 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A238" s="2" t="s">
+    <row r="238" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A238" s="20" t="s">
         <v>641</v>
       </c>
       <c r="B238" s="2" t="s">
@@ -38660,7 +38679,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="48" hidden="1">
+    <row r="239" spans="1:4" ht="60">
       <c r="A239" s="2" t="s">
         <v>650</v>
       </c>
@@ -38674,8 +38693,8 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="15.75" hidden="1" customHeight="1">
-      <c r="A240" s="2" t="s">
+    <row r="240" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A240" s="20" t="s">
         <v>625</v>
       </c>
       <c r="B240" s="2" t="s">
@@ -40161,52 +40180,55 @@
   <autoFilter ref="A1:H310" xr:uid="{00000000-0009-0000-0000-000006000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="ADLBC.A1HI"/>
-        <filter val="ADLBC.A1LO"/>
-        <filter val="ADLBC.ABLFL"/>
-        <filter val="ADLBC.ADT"/>
-        <filter val="ADLBC.ADY"/>
-        <filter val="ADLBC.AENTMTFL"/>
-        <filter val="ADLBC.AGE"/>
-        <filter val="ADLBC.AGEGR1"/>
-        <filter val="ADLBC.AGEGR1N"/>
-        <filter val="ADLBC.ALBTRVAL"/>
-        <filter val="ADLBC.ANL01FL"/>
-        <filter val="ADLBC.ANRIND"/>
-        <filter val="ADLBC.AVAL"/>
-        <filter val="ADLBC.AVISIT"/>
-        <filter val="ADLBC.AVISITN"/>
-        <filter val="ADLBC.BASE"/>
-        <filter val="ADLBC.BNRIND"/>
-        <filter val="ADLBC.BR2A1HI"/>
-        <filter val="ADLBC.BR2A1LO"/>
-        <filter val="ADLBC.CHG"/>
-        <filter val="ADLBC.COMP24FL"/>
-        <filter val="ADLBC.DSRAEFL"/>
-        <filter val="ADLBC.LBNRIND"/>
-        <filter val="ADLBC.LBSEQ"/>
-        <filter val="ADLBC.LBSTRESN"/>
-        <filter val="ADLBC.PARAM"/>
-        <filter val="ADLBC.PARAMCD"/>
-        <filter val="ADLBC.PARAMN"/>
-        <filter val="ADLBC.PARCAT1"/>
-        <filter val="ADLBC.R2A1HI"/>
-        <filter val="ADLBC.R2A1LO"/>
-        <filter val="ADLBC.RACE"/>
-        <filter val="ADLBC.RACEN"/>
-        <filter val="ADLBC.SAFFL"/>
-        <filter val="ADLBC.SEX"/>
-        <filter val="ADLBC.STUDYID"/>
-        <filter val="ADLBC.SUBJID"/>
-        <filter val="ADLBC.TRTA"/>
-        <filter val="ADLBC.TRTAN"/>
-        <filter val="ADLBC.TRTEDT"/>
-        <filter val="ADLBC.TRTP"/>
-        <filter val="ADLBC.TRTPN"/>
-        <filter val="ADLBC.TRTSDT"/>
-        <filter val="ADLBC.USUBJID"/>
-        <filter val="ADLBC.VISIT"/>
-        <filter val="ADLBC.VISITNUM"/>
+        <filter val="ADSL.AGE"/>
+        <filter val="ADSL.AGEGR1"/>
+        <filter val="ADSL.AGEGR1N"/>
+        <filter val="ADSL.AGEU"/>
+        <filter val="ADSL.ARM"/>
+        <filter val="ADSL.AVGDD"/>
+        <filter val="ADSL.BMIBL"/>
+        <filter val="ADSL.BMIBLGR1"/>
+        <filter val="ADSL.COMP16FL"/>
+        <filter val="ADSL.COMP24FL"/>
+        <filter val="ADSL.COMP8FL"/>
+        <filter val="ADSL.CUMDOSE"/>
+        <filter val="ADSL.DCDECOD"/>
+        <filter val="ADSL.DCREASCD"/>
+        <filter val="ADSL.DISCONFL"/>
+        <filter val="ADSL.DISONSDT"/>
+        <filter val="ADSL.DSRAEFL"/>
+        <filter val="ADSL.DTHFL"/>
+        <filter val="ADSL.DURDIS"/>
+        <filter val="ADSL.DURDSGR1"/>
+        <filter val="ADSL.EDUCLVL"/>
+        <filter val="ADSL.EFFFL"/>
+        <filter val="ADSL.EOSSTT"/>
+        <filter val="ADSL.ETHNIC"/>
+        <filter val="ADSL.HEIGHTBL"/>
+        <filter val="ADSL.ITTFL"/>
+        <filter val="ADSL.MMSETOT"/>
+        <filter val="ADSL.RACE"/>
+        <filter val="ADSL.RACEN"/>
+        <filter val="ADSL.RFENDT"/>
+        <filter val="ADSL.RFENDTC"/>
+        <filter val="ADSL.RFSTDTC"/>
+        <filter val="ADSL.SAFFL"/>
+        <filter val="ADSL.SEX"/>
+        <filter val="ADSL.SITEGR1"/>
+        <filter val="ADSL.SITEID"/>
+        <filter val="ADSL.STUDYID"/>
+        <filter val="ADSL.SUBJID"/>
+        <filter val="ADSL.TRT01A"/>
+        <filter val="ADSL.TRT01AN"/>
+        <filter val="ADSL.TRT01P"/>
+        <filter val="ADSL.TRT01PN"/>
+        <filter val="ADSL.TRTDUR"/>
+        <filter val="ADSL.TRTEDT"/>
+        <filter val="ADSL.TRTSDT"/>
+        <filter val="ADSL.USUBJID"/>
+        <filter val="ADSL.VISIT1DT"/>
+        <filter val="ADSL.VISNUMEN"/>
+        <filter val="ADSL.WEIGHTBL"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -40230,18 +40252,18 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="6.5" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="45.83203125" customWidth="1"/>
-    <col min="6" max="6" width="44.83203125" customWidth="1"/>
-    <col min="7" max="29" width="45.6640625" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" customWidth="1"/>
+    <col min="7" max="29" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="48">
+    <row r="1" spans="1:29" ht="45">
       <c r="A1" s="6" t="s">
         <v>1594</v>
       </c>
@@ -40284,7 +40306,7 @@
       <c r="AB1" s="8"/>
       <c r="AC1" s="8"/>
     </row>
-    <row r="2" spans="1:29" ht="196">
+    <row r="2" spans="1:29" ht="200.25">
       <c r="A2" s="8" t="s">
         <v>1599</v>
       </c>
@@ -40626,7 +40648,7 @@
       <c r="AB9" s="8"/>
       <c r="AC9" s="8"/>
     </row>
-    <row r="10" spans="1:29" ht="32">
+    <row r="10" spans="1:29" ht="30">
       <c r="A10" s="15" t="s">
         <v>1635</v>
       </c>
@@ -40669,7 +40691,7 @@
       <c r="AB10" s="8"/>
       <c r="AC10" s="8"/>
     </row>
-    <row r="11" spans="1:29" ht="144">
+    <row r="11" spans="1:29" ht="135">
       <c r="A11" s="15" t="s">
         <v>1635</v>
       </c>
@@ -71389,12 +71411,12 @@
       <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="62.5" customWidth="1"/>
-    <col min="3" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>